<commit_message>
Finished E-Glass linear optimization & postprocessing
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PMMA_const_full" sheetId="1" r:id="rId1"/>
     <sheet name="PMMA_const_hybrid" sheetId="2" r:id="rId2"/>
     <sheet name="PMMA_linear_full" sheetId="3" r:id="rId3"/>
     <sheet name="PMMA_linear_hybrid" sheetId="4" r:id="rId4"/>
+    <sheet name="E_Glass_const_full" sheetId="5" r:id="rId5"/>
+    <sheet name="E_Glass_linear_full" sheetId="6" r:id="rId6"/>
+    <sheet name="E_Glass_linear_hybrid" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="26">
   <si>
     <t>Input parameters</t>
   </si>
@@ -98,6 +101,9 @@
   <si>
     <t>Hybrid error (%)</t>
   </si>
+  <si>
+    <t>ρv, ρc, εc fixed</t>
+  </si>
 </sst>
 </file>
 
@@ -139,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -175,11 +181,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -189,6 +206,10 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +493,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="A1:F18"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,4 +1650,1080 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2140000000000</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(C2-B2)/B2</f>
+        <v>8.5470085470085472E-2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1650000000000</v>
+      </c>
+      <c r="F2" s="4">
+        <f>ABS(E2-B2)/B2</f>
+        <v>0.29487179487179488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>180000</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D18" si="0">ABS(C3-B3)/B3</f>
+        <v>5.5248618784530384E-3</v>
+      </c>
+      <c r="E3" s="3">
+        <v>130000</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F19" si="1">ABS(E3-B3)/B3</f>
+        <v>0.28176795580110497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.02</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="E4">
+        <v>2.2970000000000002</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="1"/>
+        <v>1.2970000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C5">
+        <v>100556.7</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>5.5669999999999713E-3</v>
+      </c>
+      <c r="E5">
+        <v>178066.2</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.78066200000000008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C6">
+        <v>0.30030000000000001</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>1.000000000000075E-3</v>
+      </c>
+      <c r="E6">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
+        <v>2.1166666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C8">
+        <v>1505.924</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>3.9493333333333186E-3</v>
+      </c>
+      <c r="E8">
+        <v>5276.66</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
+        <v>2.5177733333333334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.2</v>
+      </c>
+      <c r="C10">
+        <v>0.19750000000000001</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2500000000000011E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.27000000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1100</v>
+      </c>
+      <c r="C12">
+        <v>1050.6890000000001</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4828181818181746E-2</v>
+      </c>
+      <c r="E12">
+        <v>405.58</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.63129090909090912</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1683</v>
+      </c>
+      <c r="C14">
+        <v>1683</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1683</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1235</v>
+      </c>
+      <c r="C15">
+        <v>1235</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1235</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.94</v>
+      </c>
+      <c r="C16">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2553191489360558E-3</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>6.3829787234042618E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0.94</v>
+      </c>
+      <c r="C17">
+        <v>0.94</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0.94</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C18">
+        <v>10198</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="E18">
+        <v>2500.1799999999998</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="1"/>
+        <v>0.74998199999999993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(C2-B2)/B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>834000000000</v>
+      </c>
+      <c r="F2" s="4">
+        <f>ABS(E2-B2)/B2</f>
+        <v>0.64358974358974363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>181000</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D18" si="0">ABS(C3-B3)/B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>124000</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F6" si="1">ABS(E3-B3)/B3</f>
+        <v>0.31491712707182318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9999999999998916E-3</v>
+      </c>
+      <c r="E4">
+        <v>1.91517409145302</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.91517409145301998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C5">
+        <v>99441.7</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>5.5830000000000289E-3</v>
+      </c>
+      <c r="E5">
+        <v>207434.67318667899</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0743467318667899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C6">
+        <v>0.3029</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9166666666666657E-2</v>
+      </c>
+      <c r="E6">
+        <v>1.0851294576884201</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
+        <v>2.4779790310526284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4.3956999999999999E-5</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>2.1112372304199919E-3</v>
+      </c>
+      <c r="E7">
+        <v>1.76158773137132E-4</v>
+      </c>
+      <c r="F7" s="4">
+        <f>ABS(E7-B7)/B7</f>
+        <v>2.9990640893787055</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C8">
+        <v>1060.3599999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8185185185185276E-2</v>
+      </c>
+      <c r="E8">
+        <v>4057.9485813880101</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" ref="F3:F18" si="2">ABS(E8-B8)/B8</f>
+        <v>2.7573597975814907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C9">
+        <v>4.3740000000000001E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2300884955752125E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.167671314994226</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="2"/>
+        <v>2.7095423671288943</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C10">
+        <v>9.3515551372699998E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4588499760800844E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.174443889549037</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.83818640199196004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C11">
+        <v>2.7732053942500001E-4</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0068765282685457E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7.0785421626685802E-5</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.74987483524139298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1041</v>
+      </c>
+      <c r="C12">
+        <v>1040.9460128600001</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>5.1860845340912709E-5</v>
+      </c>
+      <c r="E12">
+        <v>935.42130914199402</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.10142045231316617</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.25121553113599998</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>3.0055864339768444E-2</v>
+      </c>
+      <c r="E13">
+        <v>6.4906487703679697E-2</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.74939580037189313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1683</v>
+      </c>
+      <c r="C14">
+        <v>1683</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1683</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1235</v>
+      </c>
+      <c r="C15">
+        <v>1235</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1235</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.94</v>
+      </c>
+      <c r="C16">
+        <v>0.92424733081199995</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>1.67581587106383E-2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="2"/>
+        <v>6.3829787234042618E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0.94</v>
+      </c>
+      <c r="C17">
+        <v>0.94</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0.94</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C18">
+        <v>10287.681002900001</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>2.8768100290000074E-2</v>
+      </c>
+      <c r="E18">
+        <v>21698.9566843385</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="2"/>
+        <v>1.16989566843385</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2190000000000</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(C2-B2)/B2</f>
+        <v>6.4102564102564097E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>178000</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D18" si="0">ABS(C3-B3)/B3</f>
+        <v>1.6574585635359115E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C5">
+        <v>111505</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.11505</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C6">
+        <v>0.27004725294725701</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.13446393286135574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C7">
+        <v>1.6881454492321399E-4</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>2.8323392718096256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C8">
+        <v>1174.21212764968</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>8.723345152748152E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C9">
+        <v>4.2441927831543498E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>6.101929576231193E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.20162626119914101</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1246181369772499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C11">
+        <v>1.80065138801791E-4</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.36372742472865371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1041</v>
+      </c>
+      <c r="C12">
+        <v>1355.34087825149</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.30196049784004808</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.26127436085031103</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>8.7813160243668687E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1683</v>
+      </c>
+      <c r="C14">
+        <v>1683</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1235</v>
+      </c>
+      <c r="C15">
+        <v>1235</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.94</v>
+      </c>
+      <c r="C16">
+        <v>0.95818661567533403</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>1.9347463484397961E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0.94</v>
+      </c>
+      <c r="C17">
+        <v>0.94</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C18">
+        <v>25483.1978584149</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5483197858414901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PMMA all simulation and figures
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PMMA_const_full" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +799,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,7 +2666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
comparison of multi reaction hybrid and 2 heat flux curves
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="PMMA_const_full" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,8 @@
     <sheet name="E_Glass_linear_full" sheetId="6" r:id="rId7"/>
     <sheet name="E_Glass_linear_hybrid" sheetId="7" r:id="rId8"/>
     <sheet name="E_Glass_linear_full_2mass" sheetId="9" r:id="rId9"/>
+    <sheet name="E_Glass_linear_full_mass_fbtemp" sheetId="10" r:id="rId10"/>
+    <sheet name="multiReactionCharringHybrid" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="26">
   <si>
     <t>Input parameters</t>
   </si>
@@ -795,6 +797,295 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3430000000000</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(C2-B2)/B2</f>
+        <v>0.46581196581196582</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>183000</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D18" si="0">ABS(C3-B3)/B3</f>
+        <v>1.1049723756906077E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999901E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C5">
+        <v>99847.5</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5250000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C6">
+        <v>0.313</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2051282051282081E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4.2400000000000001E-5</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>3.7457434733257647E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C8">
+        <v>1082.2</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0370370370370794E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C9">
+        <v>4.5760000000000002E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2389380530973562E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C10">
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.12118018967334032</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>6.00706713780918E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1041</v>
+      </c>
+      <c r="C12">
+        <v>1045</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>3.8424591738712775E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.25650000000000001</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>9.652509652509661E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1683</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1235</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.94</v>
+      </c>
+      <c r="C16">
+        <v>0.941716</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8255319148936713E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0.94</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C18">
+        <v>10246.6</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>2.4660000000000036E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
@@ -2963,8 +3254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3012,7 +3303,7 @@
         <v>183000</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D19" si="0">ABS(C3-B3)/B3</f>
+        <f t="shared" ref="D3:D18" si="0">ABS(C3-B3)/B3</f>
         <v>1.1049723756906077E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2 Mass + TGA
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="46">
   <si>
     <t>Input parameters</t>
   </si>
@@ -152,9 +152,6 @@
     <t>1 Mass + DSC + B Temp</t>
   </si>
   <si>
-    <t>X/O</t>
-  </si>
-  <si>
     <t>1 Mass</t>
   </si>
   <si>
@@ -164,7 +161,13 @@
     <t>Single reaction non-charring with ignition</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Three reactions charring</t>
+  </si>
+  <si>
+    <t>10 kW X/100 kW O</t>
+  </si>
+  <si>
+    <t>2 Mass + TGA</t>
   </si>
 </sst>
 </file>
@@ -258,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -271,6 +274,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,31 +564,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -595,10 +607,16 @@
       <c r="D2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>35</v>
@@ -606,11 +624,15 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -620,11 +642,15 @@
       <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -634,32 +660,52 @@
       <c r="C5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -667,7 +713,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -675,7 +721,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -683,13 +729,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -697,19 +743,30 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
finished 2 reactions 3 mass
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="E_Glass_linear_full_mass_fbtemp" sheetId="10" r:id="rId11"/>
     <sheet name="multiReactionCharringHybrid" sheetId="11" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="47">
   <si>
     <t>Input parameters</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>2 Mass + TGA</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -274,6 +277,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,7 +573,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,18 +587,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -630,7 +636,9 @@
       <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -648,7 +656,9 @@
       <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -684,7 +694,9 @@
       <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -696,6 +708,12 @@
       <c r="C7" t="s">
         <v>45</v>
       </c>
+      <c r="D7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -704,6 +722,9 @@
       <c r="B8" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -730,10 +751,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
new 2 reactions 2 temp case
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="E_Glass_linear_full_mass_fbtemp" sheetId="10" r:id="rId11"/>
     <sheet name="multiReactionCharringHybrid" sheetId="11" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="47">
   <si>
     <t>Input parameters</t>
   </si>
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -277,6 +277,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -573,7 +576,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,18 +590,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="10"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -637,7 +640,7 @@
         <v>26</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -657,7 +660,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -670,9 +673,7 @@
       <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="D5" s="8"/>
       <c r="E5" t="s">
         <v>32</v>
       </c>
@@ -714,6 +715,9 @@
       <c r="E7" t="s">
         <v>28</v>
       </c>
+      <c r="F7" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -725,6 +729,9 @@
       <c r="C8" t="s">
         <v>28</v>
       </c>
+      <c r="D8" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -751,10 +758,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
post processing and modified cases
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="47">
   <si>
     <t>Input parameters</t>
   </si>
@@ -155,9 +155,6 @@
     <t>1 Mass</t>
   </si>
   <si>
-    <t>X?</t>
-  </si>
-  <si>
     <t>Single reaction non-charring with ignition</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>running</t>
   </si>
 </sst>
 </file>
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -277,6 +277,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -573,10 +576,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,18 +596,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -633,8 +639,8 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>44</v>
+      <c r="D3" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -654,7 +660,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -673,11 +679,15 @@
       <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="E5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -690,13 +700,13 @@
         <v>37</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -707,10 +717,10 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>28</v>
@@ -724,13 +734,13 @@
         <v>36</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -758,10 +768,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="11"/>
+      <c r="A13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="12"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -797,7 +807,7 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="99" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
summary 1 reaction results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -23,7 +24,7 @@
     <sheet name="E_Glass_linear_full_mass_fbtemp" sheetId="10" r:id="rId14"/>
     <sheet name="multiReactionCharringHybrid" sheetId="11" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="80">
   <si>
     <t>Input parameters</t>
   </si>
@@ -213,6 +214,66 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>running_home</t>
+  </si>
+  <si>
+    <t>running_office</t>
+  </si>
+  <si>
+    <t>Xi</t>
+  </si>
+  <si>
+    <t>1 Mass + FT + BT</t>
+  </si>
+  <si>
+    <t>1 Mass + BT</t>
+  </si>
+  <si>
+    <t>1 Mass + TGA + BT</t>
+  </si>
+  <si>
+    <t>1 Mass + DSC + BT</t>
+  </si>
+  <si>
+    <t>1 Mass + FT</t>
+  </si>
+  <si>
+    <t>1 Mass + TGA + FT</t>
+  </si>
+  <si>
+    <t>[6.38% 299.91%]</t>
+  </si>
+  <si>
+    <t>[0.88% 283.23%]</t>
+  </si>
+  <si>
+    <t>[0% 230.97%]</t>
+  </si>
+  <si>
+    <t>[0% 177.43%]</t>
+  </si>
+  <si>
+    <t>[0.15% 46.58%]</t>
+  </si>
+  <si>
+    <t>[0% 230.53%]</t>
+  </si>
+  <si>
+    <t>[0% 72.39%]</t>
+  </si>
+  <si>
+    <t>[0.45% 287.61%]</t>
+  </si>
+  <si>
+    <t>[2.21% 297.28%]</t>
+  </si>
+  <si>
+    <t>[0.5% 158.17%]</t>
+  </si>
+  <si>
+    <t>[0.16% 203.76%]</t>
   </si>
 </sst>
 </file>
@@ -320,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -333,6 +394,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -647,7 +711,10 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,15 +732,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -702,6 +769,12 @@
       <c r="A3" t="s">
         <v>39</v>
       </c>
+      <c r="B3" s="4">
+        <v>1.2545999999999999</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
       <c r="G3" s="7" t="s">
         <v>34</v>
       </c>
@@ -710,6 +783,12 @@
       <c r="A4" t="s">
         <v>26</v>
       </c>
+      <c r="B4" s="4">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
       <c r="G4" s="7" t="s">
         <v>30</v>
       </c>
@@ -718,6 +797,12 @@
       <c r="A5" t="s">
         <v>27</v>
       </c>
+      <c r="B5" s="4">
+        <v>0.36809999999999998</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
       <c r="G5" s="7" t="s">
         <v>30</v>
       </c>
@@ -726,6 +811,12 @@
       <c r="A6" t="s">
         <v>28</v>
       </c>
+      <c r="B6" s="4">
+        <v>0.27350000000000002</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
       <c r="G6" s="7" t="s">
         <v>30</v>
       </c>
@@ -734,6 +825,12 @@
       <c r="A7" t="s">
         <v>31</v>
       </c>
+      <c r="B7" s="4">
+        <v>5.4800000000000001E-2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
       <c r="G7" s="7" t="s">
         <v>30</v>
       </c>
@@ -742,6 +839,12 @@
       <c r="A8" t="s">
         <v>48</v>
       </c>
+      <c r="B8" s="4">
+        <v>0.47689999999999999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
       <c r="G8" s="12" t="s">
         <v>44</v>
       </c>
@@ -750,6 +853,12 @@
       <c r="A9" t="s">
         <v>35</v>
       </c>
+      <c r="B9" s="4">
+        <v>0.1825</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
       <c r="G9" s="7" t="s">
         <v>30</v>
       </c>
@@ -758,6 +867,12 @@
       <c r="A10" t="s">
         <v>36</v>
       </c>
+      <c r="B10" s="4">
+        <v>0.66779999999999995</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
       <c r="G10" s="7" t="s">
         <v>30</v>
       </c>
@@ -766,6 +881,12 @@
       <c r="A11" t="s">
         <v>37</v>
       </c>
+      <c r="B11" s="4">
+        <v>0.66610000000000003</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
       <c r="G11" s="7" t="s">
         <v>34</v>
       </c>
@@ -774,6 +895,12 @@
       <c r="A12" t="s">
         <v>38</v>
       </c>
+      <c r="B12" s="4">
+        <v>0.32590000000000002</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
       <c r="G12" s="7" t="s">
         <v>44</v>
       </c>
@@ -782,6 +909,12 @@
       <c r="A13" t="s">
         <v>47</v>
       </c>
+      <c r="B13" s="4">
+        <v>0.29320000000000002</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
       <c r="G13" s="12" t="s">
         <v>44</v>
       </c>
@@ -795,15 +928,15 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -853,15 +986,15 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -951,15 +1084,15 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1005,7 +1138,7 @@
         <v>43</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1021,15 +1154,15 @@
         <v>54</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>55</v>
       </c>
-      <c r="G37" s="13" t="s">
-        <v>56</v>
+      <c r="G37" s="14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1044,8 +1177,8 @@
       <c r="A39" t="s">
         <v>36</v>
       </c>
-      <c r="G39" s="8" t="s">
-        <v>34</v>
+      <c r="G39" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1080,6 +1213,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1331,6 +1465,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E19"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1741,8 +1876,9 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2037,8 +2173,9 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2313,8 +2450,9 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2590,6 +2728,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="O33" sqref="O33"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2599,10 +2738,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F227" sqref="F227"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="1">
+      <selection activeCell="G185" sqref="G185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,12 +2753,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2822,10 +2964,7 @@
       <c r="C15">
         <v>1683</v>
       </c>
-      <c r="D15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -2837,10 +2976,7 @@
       <c r="C16">
         <v>1235</v>
       </c>
-      <c r="D16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -2867,38 +3003,3078 @@
       <c r="C18">
         <v>0.94</v>
       </c>
-      <c r="D18" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="C19">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="3">
         <v>10000</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>21698.9566843385</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D20" s="4">
         <f t="shared" si="0"/>
         <v>1.16989566843385</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="4">
-        <f>AVERAGE(D3:D19)</f>
-        <v>1.0332103485123176</v>
+      <c r="D21" s="4">
+        <f>AVERAGE(D3:D20)</f>
+        <v>1.2546125660506713</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+    </row>
+    <row r="23" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2190000000000</v>
+      </c>
+      <c r="D24" s="4">
+        <f>ABS(C24-B24)/B24</f>
+        <v>6.4102564102564097E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C25" s="3">
+        <v>178000</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" ref="D25:D41" si="1">ABS(C25-B25)/B25</f>
+        <v>1.6574585635359115E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="1"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C27">
+        <v>111505</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="1"/>
+        <v>0.11505</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C28">
+        <v>0.27004725294725701</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13446393286135574</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C29">
+        <v>1.6881454492321399E-4</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="1"/>
+        <v>2.8323392718096256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C30">
+        <v>1174.21212764968</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="1"/>
+        <v>8.723345152748152E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C31">
+        <v>4.2441927831543498E-2</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="1"/>
+        <v>6.101929576231193E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C32">
+        <v>0.20162626119914101</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="1"/>
+        <v>1.1246181369772499</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C33">
+        <v>1.80065138801791E-4</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="1"/>
+        <v>0.36372742472865371</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>1041</v>
+      </c>
+      <c r="C34">
+        <v>1355.34087825149</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="1"/>
+        <v>0.30196049784004808</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C35">
+        <v>0.26127436085031103</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>8.7813160243668687E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36">
+        <v>1683</v>
+      </c>
+      <c r="C36">
+        <v>1683</v>
+      </c>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>1235</v>
+      </c>
+      <c r="C37">
+        <v>1235</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>0.94</v>
+      </c>
+      <c r="C38">
+        <v>0.95818661567533403</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" ref="D38:D42" si="2">ABS(C38-B38)/B38</f>
+        <v>1.9347463484397961E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <v>0.94</v>
+      </c>
+      <c r="C39">
+        <v>0.94</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="C40">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C41">
+        <v>25483.1978584149</v>
+      </c>
+      <c r="D41" s="4">
+        <f>ABS(C41-B41)/B41</f>
+        <v>1.5483197858414901</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="4">
+        <f>AVERAGE(D24:D41)</f>
+        <v>0.47803840904249323</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+    </row>
+    <row r="44" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C45" s="3">
+        <v>3300000000000</v>
+      </c>
+      <c r="D45" s="4">
+        <f>ABS(C45-B45)/B45</f>
+        <v>0.41025641025641024</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C46" s="3">
+        <v>183000</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" ref="D46:D62" si="3">ABS(C46-B46)/B46</f>
+        <v>1.1049723756906077E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C48">
+        <v>101238.39999999999</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="3"/>
+        <v>1.2383999999999942E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C49">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="3"/>
+        <v>6.4102564102564166E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C50" s="3">
+        <v>8.933E-5</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" si="3"/>
+        <v>1.027922814982974</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C51">
+        <v>1040.77</v>
+      </c>
+      <c r="D51" s="4">
+        <f t="shared" si="3"/>
+        <v>3.6324074074074092E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C52">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="D52" s="4">
+        <f t="shared" si="3"/>
+        <v>2.309734513274337</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C53">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="D53" s="4">
+        <f t="shared" si="3"/>
+        <v>0.19915700737618547</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C54">
+        <v>3.1700000000000001E-4</v>
+      </c>
+      <c r="D54" s="4">
+        <f t="shared" si="3"/>
+        <v>0.12014134275618379</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55">
+        <v>1041</v>
+      </c>
+      <c r="C55">
+        <v>1172</v>
+      </c>
+      <c r="D55" s="4">
+        <f t="shared" si="3"/>
+        <v>0.12584053794428435</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C56">
+        <v>0.1143</v>
+      </c>
+      <c r="D56" s="4">
+        <f t="shared" si="3"/>
+        <v>0.55868725868725866</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57">
+        <v>1683</v>
+      </c>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58">
+        <v>1235</v>
+      </c>
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59">
+        <v>0.94</v>
+      </c>
+      <c r="C59">
+        <v>0.94240000000000002</v>
+      </c>
+      <c r="D59" s="4">
+        <f t="shared" ref="D59:D63" si="4">ABS(C59-B59)/B59</f>
+        <v>2.5531914893617753E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60">
+        <v>0.94</v>
+      </c>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C62">
+        <v>12751</v>
+      </c>
+      <c r="D62" s="4">
+        <f>ABS(C62-B62)/B62</f>
+        <v>0.27510000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="4">
+        <f>AVERAGE(D45:D62)</f>
+        <v>0.3680895313357529</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+    </row>
+    <row r="65" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C66" s="3">
+        <v>3320000000000</v>
+      </c>
+      <c r="D66" s="4">
+        <f>ABS(C66-B66)/B66</f>
+        <v>0.41880341880341881</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C67" s="3">
+        <v>183000</v>
+      </c>
+      <c r="D67" s="4">
+        <f t="shared" ref="D67:D83" si="5">ABS(C67-B67)/B67</f>
+        <v>1.1049723756906077E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>1.008</v>
+      </c>
+      <c r="D68" s="4">
+        <f t="shared" si="5"/>
+        <v>8.0000000000000071E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C69">
+        <v>100484</v>
+      </c>
+      <c r="D69" s="4">
+        <f t="shared" si="5"/>
+        <v>4.8399999999999997E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C70">
+        <v>0.29220000000000002</v>
+      </c>
+      <c r="D70" s="4">
+        <f t="shared" si="5"/>
+        <v>6.3461538461538416E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C71" s="3">
+        <v>8.4629999999999994E-5</v>
+      </c>
+      <c r="D71" s="4">
+        <f t="shared" si="5"/>
+        <v>0.92122587968217917</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C72">
+        <v>1047.5</v>
+      </c>
+      <c r="D72" s="4">
+        <f t="shared" si="5"/>
+        <v>3.0092592592592591E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C73">
+        <v>0.12540000000000001</v>
+      </c>
+      <c r="D73" s="4">
+        <f t="shared" si="5"/>
+        <v>1.7743362831858414</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C74">
+        <v>9.6100000000000005E-2</v>
+      </c>
+      <c r="D74" s="4">
+        <f t="shared" si="5"/>
+        <v>1.2644889357218194E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C75">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="D75" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76">
+        <v>1041</v>
+      </c>
+      <c r="C76">
+        <v>1053.3699999999999</v>
+      </c>
+      <c r="D76" s="4">
+        <f t="shared" si="5"/>
+        <v>1.1882804995196821E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C77">
+        <v>0.24160000000000001</v>
+      </c>
+      <c r="D77" s="4">
+        <f t="shared" si="5"/>
+        <v>6.7181467181467169E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78">
+        <v>1683</v>
+      </c>
+      <c r="D78" s="4"/>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>1235</v>
+      </c>
+      <c r="D79" s="4"/>
+    </row>
+    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80">
+        <v>0.94</v>
+      </c>
+      <c r="C80">
+        <v>0.94159999999999999</v>
+      </c>
+      <c r="D80" s="4">
+        <f t="shared" ref="D80:D84" si="6">ABS(C80-B80)/B80</f>
+        <v>1.7021276595745169E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81">
+        <v>0.94</v>
+      </c>
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B82">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D82" s="4"/>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C83">
+        <v>4956.6000000000004</v>
+      </c>
+      <c r="D83" s="4">
+        <f>ABS(C83-B83)/B83</f>
+        <v>0.50434000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D84" s="4">
+        <f>AVERAGE(D66:D83)</f>
+        <v>0.27354005183399521</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
+    </row>
+    <row r="86" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C87" s="3">
+        <v>3430000000000</v>
+      </c>
+      <c r="D87" s="4">
+        <f>ABS(C87-B87)/B87</f>
+        <v>0.46581196581196582</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C88" s="3">
+        <v>183000</v>
+      </c>
+      <c r="D88" s="4">
+        <f t="shared" ref="D88:D104" si="7">ABS(C88-B88)/B88</f>
+        <v>1.1049723756906077E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="D89" s="4">
+        <f t="shared" si="7"/>
+        <v>1.2999999999999901E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C90">
+        <v>99847.5</v>
+      </c>
+      <c r="D90" s="4">
+        <f t="shared" si="7"/>
+        <v>1.5250000000000001E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C91">
+        <v>0.313</v>
+      </c>
+      <c r="D91" s="4">
+        <f t="shared" si="7"/>
+        <v>3.2051282051282081E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C92" s="3">
+        <v>4.2400000000000001E-5</v>
+      </c>
+      <c r="D92" s="4">
+        <f t="shared" si="7"/>
+        <v>3.7457434733257647E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B93" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C93">
+        <v>1082.2</v>
+      </c>
+      <c r="D93" s="4">
+        <f t="shared" si="7"/>
+        <v>2.0370370370370794E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C94">
+        <v>4.5760000000000002E-2</v>
+      </c>
+      <c r="D94" s="4">
+        <f t="shared" si="7"/>
+        <v>1.2389380530973562E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C95">
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="D95" s="4">
+        <f t="shared" si="7"/>
+        <v>0.12118018967334032</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C96">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D96" s="4">
+        <f t="shared" si="7"/>
+        <v>6.00706713780918E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97">
+        <v>1041</v>
+      </c>
+      <c r="C97">
+        <v>1045</v>
+      </c>
+      <c r="D97" s="4">
+        <f t="shared" si="7"/>
+        <v>3.8424591738712775E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C98">
+        <v>0.25650000000000001</v>
+      </c>
+      <c r="D98" s="4">
+        <f t="shared" si="7"/>
+        <v>9.652509652509661E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B99">
+        <v>1683</v>
+      </c>
+      <c r="D99" s="4"/>
+    </row>
+    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B100">
+        <v>1235</v>
+      </c>
+      <c r="D100" s="4"/>
+    </row>
+    <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B101">
+        <v>0.94</v>
+      </c>
+      <c r="C101">
+        <v>0.941716</v>
+      </c>
+      <c r="D101" s="4">
+        <f t="shared" ref="D101:D105" si="8">ABS(C101-B101)/B101</f>
+        <v>1.8255319148936713E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B102">
+        <v>0.94</v>
+      </c>
+      <c r="D102" s="4"/>
+    </row>
+    <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B103">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D103" s="4"/>
+    </row>
+    <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C104">
+        <v>10246.6</v>
+      </c>
+      <c r="D104" s="4">
+        <f>ABS(C104-B104)/B104</f>
+        <v>2.4660000000000036E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D105" s="4">
+        <f>AVERAGE(D87:D104)</f>
+        <v>5.4836216561998219E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B106" s="16"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="16"/>
+    </row>
+    <row r="107" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B108" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C108" s="3">
+        <v>2400000000000</v>
+      </c>
+      <c r="D108" s="4">
+        <f>ABS(C108-B108)/B108</f>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C109" s="3">
+        <v>181000</v>
+      </c>
+      <c r="D109" s="4">
+        <f t="shared" ref="D109:D125" si="9">ABS(C109-B109)/B109</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>1.00576</v>
+      </c>
+      <c r="D110" s="4">
+        <f t="shared" si="9"/>
+        <v>5.7599999999999874E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C111">
+        <v>99269</v>
+      </c>
+      <c r="D111" s="4">
+        <f t="shared" si="9"/>
+        <v>7.3099999999999997E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C112">
+        <v>0.28050000000000003</v>
+      </c>
+      <c r="D112" s="4">
+        <f t="shared" si="9"/>
+        <v>0.10096153846153837</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C113" s="3">
+        <v>9.4487000000000005E-5</v>
+      </c>
+      <c r="D113" s="4">
+        <f t="shared" si="9"/>
+        <v>1.1449943246311012</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C114">
+        <v>1020.9</v>
+      </c>
+      <c r="D114" s="4">
+        <f t="shared" si="9"/>
+        <v>5.4722222222222242E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C115">
+        <v>0.14940000000000001</v>
+      </c>
+      <c r="D115" s="4">
+        <f t="shared" si="9"/>
+        <v>2.3053097345132749</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B116">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C116">
+        <v>0.2228</v>
+      </c>
+      <c r="D116" s="4">
+        <f t="shared" si="9"/>
+        <v>1.3477344573234986</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C117" s="3">
+        <v>8.3590000000000004E-5</v>
+      </c>
+      <c r="D117" s="4">
+        <f t="shared" si="9"/>
+        <v>0.70462897526501767</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B118">
+        <v>1041</v>
+      </c>
+      <c r="C118">
+        <v>878.6</v>
+      </c>
+      <c r="D118" s="4">
+        <f t="shared" si="9"/>
+        <v>0.15600384245917384</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B119" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C119">
+        <v>0.44</v>
+      </c>
+      <c r="D119" s="4">
+        <f t="shared" si="9"/>
+        <v>0.69884169884169878</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B120">
+        <v>1683</v>
+      </c>
+      <c r="D120" s="4"/>
+    </row>
+    <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B121">
+        <v>1235</v>
+      </c>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B122">
+        <v>0.94</v>
+      </c>
+      <c r="C122">
+        <v>0.93320000000000003</v>
+      </c>
+      <c r="D122" s="4">
+        <f t="shared" ref="D122:D126" si="10">ABS(C122-B122)/B122</f>
+        <v>7.234042553191402E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B123">
+        <v>0.94</v>
+      </c>
+      <c r="D123" s="4"/>
+    </row>
+    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B124">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D124" s="4"/>
+    </row>
+    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B125" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C125">
+        <v>8825.2000000000007</v>
+      </c>
+      <c r="D125" s="4">
+        <f>ABS(C125-B125)/B125</f>
+        <v>0.11747999999999993</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D126" s="4">
+        <f>AVERAGE(D108:D125)</f>
+        <v>0.47690156156512442</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B127" s="16"/>
+      <c r="C127" s="16"/>
+      <c r="D127" s="16"/>
+    </row>
+    <row r="128" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B129" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C129" s="3">
+        <v>2130000000000</v>
+      </c>
+      <c r="D129" s="4">
+        <f>ABS(C129-B129)/B129</f>
+        <v>8.9743589743589744E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C130" s="3">
+        <v>181000</v>
+      </c>
+      <c r="D130" s="4">
+        <f t="shared" ref="D130:D146" si="11">ABS(C130-B130)/B130</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>0.99460000000000004</v>
+      </c>
+      <c r="D131" s="4">
+        <f t="shared" si="11"/>
+        <v>5.3999999999999604E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C132">
+        <v>99015</v>
+      </c>
+      <c r="D132" s="4">
+        <f t="shared" si="11"/>
+        <v>9.8499999999999994E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B133" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C133">
+        <v>0.316</v>
+      </c>
+      <c r="D133" s="4">
+        <f t="shared" si="11"/>
+        <v>1.2820512820512832E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B134" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C134" s="3">
+        <v>3.8099999999999998E-5</v>
+      </c>
+      <c r="D134" s="4">
+        <f t="shared" si="11"/>
+        <v>0.13507377979568677</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C135">
+        <v>1080.5440000000001</v>
+      </c>
+      <c r="D135" s="4">
+        <f t="shared" si="11"/>
+        <v>5.0370370370379292E-4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B136" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C136">
+        <v>6.386E-2</v>
+      </c>
+      <c r="D136" s="4">
+        <f t="shared" si="11"/>
+        <v>0.41283185840707975</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B137">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C137">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="D137" s="4">
+        <f t="shared" si="11"/>
+        <v>0.72391991570073755</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B138" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C138">
+        <v>3.7500000000000001E-4</v>
+      </c>
+      <c r="D138" s="4">
+        <f t="shared" si="11"/>
+        <v>0.32508833922261487</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B139">
+        <v>1041</v>
+      </c>
+      <c r="C139">
+        <v>960.74</v>
+      </c>
+      <c r="D139" s="4">
+        <f t="shared" si="11"/>
+        <v>7.7098943323727173E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B140" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C140">
+        <v>0.37619999999999998</v>
+      </c>
+      <c r="D140" s="4">
+        <f t="shared" si="11"/>
+        <v>0.45250965250965236</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B141">
+        <v>1683</v>
+      </c>
+      <c r="D141" s="4"/>
+    </row>
+    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B142">
+        <v>1235</v>
+      </c>
+      <c r="D142" s="4"/>
+    </row>
+    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B143">
+        <v>0.94</v>
+      </c>
+      <c r="C143">
+        <v>0.9466</v>
+      </c>
+      <c r="D143" s="4">
+        <f t="shared" ref="D143:D147" si="12">ABS(C143-B143)/B143</f>
+        <v>7.0212765957447347E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B144">
+        <v>0.94</v>
+      </c>
+      <c r="D144" s="4"/>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B145">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D145" s="4"/>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B146" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C146">
+        <v>13027</v>
+      </c>
+      <c r="D146" s="4">
+        <f>ABS(C146-B146)/B146</f>
+        <v>0.30270000000000002</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D147" s="4">
+        <f>AVERAGE(D129:D146)</f>
+        <v>0.18246868370164643</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B148" s="16"/>
+      <c r="C148" s="16"/>
+      <c r="D148" s="16"/>
+    </row>
+    <row r="149" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B150" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C150" s="3">
+        <v>2410000000000</v>
+      </c>
+      <c r="D150" s="4">
+        <f>ABS(C150-B150)/B150</f>
+        <v>2.9914529914529916E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B151" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C151" s="3">
+        <v>182000</v>
+      </c>
+      <c r="D151" s="4">
+        <f t="shared" ref="D151:D167" si="13">ABS(C151-B151)/B151</f>
+        <v>5.5248618784530384E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152">
+        <v>1.0167999999999999</v>
+      </c>
+      <c r="D152" s="4">
+        <f t="shared" si="13"/>
+        <v>1.6799999999999926E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B153" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C153">
+        <v>102453</v>
+      </c>
+      <c r="D153" s="4">
+        <f t="shared" si="13"/>
+        <v>2.453E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B154" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C154">
+        <v>0.31340000000000001</v>
+      </c>
+      <c r="D154" s="4">
+        <f t="shared" si="13"/>
+        <v>4.4871794871795267E-3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B155" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C155" s="3">
+        <v>8.9752000000000004E-5</v>
+      </c>
+      <c r="D155" s="4">
+        <f t="shared" si="13"/>
+        <v>1.0375028376844495</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B156" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C156">
+        <v>1114.96</v>
+      </c>
+      <c r="D156" s="4">
+        <f t="shared" si="13"/>
+        <v>3.2370370370370403E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B157" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C157">
+        <v>8.5550000000000001E-2</v>
+      </c>
+      <c r="D157" s="4">
+        <f t="shared" si="13"/>
+        <v>0.89269911504424793</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B158">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C158">
+        <v>3.6339999999999997E-2</v>
+      </c>
+      <c r="D158" s="4">
+        <f t="shared" si="13"/>
+        <v>0.6170706006322445</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B159" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C159">
+        <v>3.834E-4</v>
+      </c>
+      <c r="D159" s="4">
+        <f t="shared" si="13"/>
+        <v>0.3547703180212014</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B160">
+        <v>1041</v>
+      </c>
+      <c r="C160">
+        <v>440.88</v>
+      </c>
+      <c r="D160" s="4">
+        <f t="shared" si="13"/>
+        <v>0.57648414985590779</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B161" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C161">
+        <v>1.0039</v>
+      </c>
+      <c r="D161" s="4">
+        <f t="shared" si="13"/>
+        <v>2.8760617760617762</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B162">
+        <v>1683</v>
+      </c>
+      <c r="D162" s="4"/>
+    </row>
+    <row r="163" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B163">
+        <v>1235</v>
+      </c>
+      <c r="D163" s="4"/>
+    </row>
+    <row r="164" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B164">
+        <v>0.94</v>
+      </c>
+      <c r="C164">
+        <v>0.98929999999999996</v>
+      </c>
+      <c r="D164" s="4">
+        <f t="shared" ref="D164:D168" si="14">ABS(C164-B164)/B164</f>
+        <v>5.2446808510638314E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B165">
+        <v>0.94</v>
+      </c>
+      <c r="D165" s="4"/>
+    </row>
+    <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B166">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D166" s="4"/>
+    </row>
+    <row r="167" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B167" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C167">
+        <v>38288</v>
+      </c>
+      <c r="D167" s="4">
+        <f>ABS(C167-B167)/B167</f>
+        <v>2.8288000000000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D168" s="4">
+        <f>AVERAGE(D150:D167)</f>
+        <v>0.66781875339007135</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B169" s="16"/>
+      <c r="C169" s="16"/>
+      <c r="D169" s="16"/>
+    </row>
+    <row r="170" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B171" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C171" s="3">
+        <v>4320000000000</v>
+      </c>
+      <c r="D171" s="4">
+        <f>ABS(C171-B171)/B171</f>
+        <v>0.84615384615384615</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B172" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C172" s="3">
+        <v>177000</v>
+      </c>
+      <c r="D172" s="4">
+        <f t="shared" ref="D172:D188" si="15">ABS(C172-B172)/B172</f>
+        <v>2.2099447513812154E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
+      <c r="C173">
+        <v>0.94369999999999998</v>
+      </c>
+      <c r="D173" s="4">
+        <f t="shared" si="15"/>
+        <v>5.6300000000000017E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B174" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C174">
+        <v>125218.6</v>
+      </c>
+      <c r="D174" s="4">
+        <f t="shared" si="15"/>
+        <v>0.25218600000000008</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C175">
+        <v>0.20830000000000001</v>
+      </c>
+      <c r="D175" s="4">
+        <f t="shared" si="15"/>
+        <v>0.33237179487179486</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B176" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C176" s="3">
+        <v>1.75E-4</v>
+      </c>
+      <c r="D176" s="4">
+        <f t="shared" si="15"/>
+        <v>2.9727582292849037</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B177" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C177">
+        <v>1054.08</v>
+      </c>
+      <c r="D177" s="4">
+        <f t="shared" si="15"/>
+        <v>2.4000000000000066E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B178" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C178">
+        <v>4.07E-2</v>
+      </c>
+      <c r="D178" s="4">
+        <f t="shared" si="15"/>
+        <v>9.9557522123893752E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B179">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C179">
+        <v>0.09</v>
+      </c>
+      <c r="D179" s="4">
+        <f t="shared" si="15"/>
+        <v>5.1633298208640689E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B180" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C180">
+        <v>5.5999999999999995E-4</v>
+      </c>
+      <c r="D180" s="4">
+        <f t="shared" si="15"/>
+        <v>0.97879858657243801</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B181">
+        <v>1041</v>
+      </c>
+      <c r="C181">
+        <v>2525.67</v>
+      </c>
+      <c r="D181" s="4">
+        <f t="shared" si="15"/>
+        <v>1.4261959654178675</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B182" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C182">
+        <v>0.7298</v>
+      </c>
+      <c r="D182" s="4">
+        <f t="shared" si="15"/>
+        <v>1.8177606177606176</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B183">
+        <v>1683</v>
+      </c>
+      <c r="D183" s="4"/>
+    </row>
+    <row r="184" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B184">
+        <v>1235</v>
+      </c>
+      <c r="D184" s="4"/>
+    </row>
+    <row r="185" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B185">
+        <v>0.94</v>
+      </c>
+      <c r="C185">
+        <v>0.80740000000000001</v>
+      </c>
+      <c r="D185" s="4">
+        <f t="shared" ref="D185:D189" si="16">ABS(C185-B185)/B185</f>
+        <v>0.14106382978723397</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B186">
+        <v>0.94</v>
+      </c>
+      <c r="D186" s="4"/>
+    </row>
+    <row r="187" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B187">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D187" s="4"/>
+    </row>
+    <row r="188" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B188" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C188">
+        <v>13051</v>
+      </c>
+      <c r="D188" s="4">
+        <f>ABS(C188-B188)/B188</f>
+        <v>0.30509999999999998</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D189" s="4">
+        <f>AVERAGE(D171:D188)</f>
+        <v>0.66614136697821758</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B190" s="16"/>
+      <c r="C190" s="16"/>
+      <c r="D190" s="16"/>
+    </row>
+    <row r="191" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B192" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C192" s="3">
+        <v>2760000000000</v>
+      </c>
+      <c r="D192" s="4">
+        <f>ABS(C192-B192)/B192</f>
+        <v>0.17948717948717949</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B193" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C193" s="3">
+        <v>182000</v>
+      </c>
+      <c r="D193" s="4">
+        <f t="shared" ref="D193:D209" si="17">ABS(C193-B193)/B193</f>
+        <v>5.5248618784530384E-3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
+      <c r="C194">
+        <v>0.995</v>
+      </c>
+      <c r="D194" s="4">
+        <f t="shared" si="17"/>
+        <v>5.0000000000000044E-3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B195" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C195">
+        <v>101867.34</v>
+      </c>
+      <c r="D195" s="4">
+        <f t="shared" si="17"/>
+        <v>1.8673399999999965E-2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B196" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C196">
+        <v>0.30370000000000003</v>
+      </c>
+      <c r="D196" s="4">
+        <f t="shared" si="17"/>
+        <v>2.6602564102564018E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B197" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C197" s="3">
+        <v>3.5120000000000003E-5</v>
+      </c>
+      <c r="D197" s="4">
+        <f t="shared" si="17"/>
+        <v>0.20272417707150958</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B198" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C198">
+        <v>1042.5</v>
+      </c>
+      <c r="D198" s="4">
+        <f t="shared" si="17"/>
+        <v>3.4722222222222224E-2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B199" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C199">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="D199" s="4">
+        <f t="shared" si="17"/>
+        <v>3.7610619469026552E-2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B200">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C200">
+        <v>0.245</v>
+      </c>
+      <c r="D200" s="4">
+        <f t="shared" si="17"/>
+        <v>1.5816649104320339</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B201" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C201" s="3">
+        <v>7.1559999999999999E-5</v>
+      </c>
+      <c r="D201" s="4">
+        <f t="shared" si="17"/>
+        <v>0.74713780918727912</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B202">
+        <v>1041</v>
+      </c>
+      <c r="C202">
+        <v>1134.6400000000001</v>
+      </c>
+      <c r="D202" s="4">
+        <f t="shared" si="17"/>
+        <v>8.9951969260326711E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B203" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C203">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="D203" s="4">
+        <f t="shared" si="17"/>
+        <v>0.54826254826254828</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B204">
+        <v>1683</v>
+      </c>
+      <c r="D204" s="4"/>
+    </row>
+    <row r="205" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B205">
+        <v>1235</v>
+      </c>
+      <c r="D205" s="4"/>
+    </row>
+    <row r="206" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B206">
+        <v>0.94</v>
+      </c>
+      <c r="C206">
+        <v>0.91679999999999995</v>
+      </c>
+      <c r="D206" s="4">
+        <f t="shared" ref="D206:D210" si="18">ABS(C206-B206)/B206</f>
+        <v>2.4680851063829785E-2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B207">
+        <v>0.94</v>
+      </c>
+      <c r="D207" s="4"/>
+    </row>
+    <row r="208" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B208">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D208" s="4"/>
+    </row>
+    <row r="209" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B209" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C209">
+        <v>20605.599999999999</v>
+      </c>
+      <c r="D209" s="4">
+        <f>ABS(C209-B209)/B209</f>
+        <v>1.0605599999999999</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D210" s="4">
+        <f>AVERAGE(D192:D209)</f>
+        <v>0.32590022231692661</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B211" s="16"/>
+      <c r="C211" s="16"/>
+      <c r="D211" s="16"/>
+    </row>
+    <row r="212" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B213" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C213" s="3">
+        <v>2790000000000</v>
+      </c>
+      <c r="D213" s="4">
+        <f>ABS(C213-B213)/B213</f>
+        <v>0.19230769230769232</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B214" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C214" s="3">
+        <v>182000</v>
+      </c>
+      <c r="D214" s="4">
+        <f t="shared" ref="D214:D230" si="19">ABS(C214-B214)/B214</f>
+        <v>5.5248618784530384E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B215">
+        <v>1</v>
+      </c>
+      <c r="C215">
+        <v>1.0098</v>
+      </c>
+      <c r="D215" s="4">
+        <f t="shared" si="19"/>
+        <v>9.8000000000000309E-3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B216" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C216">
+        <v>99213.5</v>
+      </c>
+      <c r="D216" s="4">
+        <f t="shared" si="19"/>
+        <v>7.8650000000000005E-3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B217" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="C217">
+        <v>0.3125</v>
+      </c>
+      <c r="D217" s="4">
+        <f t="shared" si="19"/>
+        <v>1.602564102564104E-3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B218" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C218" s="3">
+        <v>4.1539999999999999E-5</v>
+      </c>
+      <c r="D218" s="4">
+        <f t="shared" si="19"/>
+        <v>5.6980703745743502E-2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B219" s="5">
+        <v>1080</v>
+      </c>
+      <c r="C219">
+        <v>1028.5999999999999</v>
+      </c>
+      <c r="D219" s="4">
+        <f t="shared" si="19"/>
+        <v>4.7592592592592679E-2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B220" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="C220">
+        <v>0.13730000000000001</v>
+      </c>
+      <c r="D220" s="4">
+        <f t="shared" si="19"/>
+        <v>2.0376106194690271</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B221">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="C221">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="D221" s="4">
+        <f t="shared" si="19"/>
+        <v>0.7502634351949421</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B222" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C222">
+        <v>3.8699999999999997E-4</v>
+      </c>
+      <c r="D222" s="4">
+        <f t="shared" si="19"/>
+        <v>0.36749116607773846</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B223">
+        <v>1041</v>
+      </c>
+      <c r="C223">
+        <v>1130.45</v>
+      </c>
+      <c r="D223" s="4">
+        <f t="shared" si="19"/>
+        <v>8.5926993275696487E-2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B224" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C224">
+        <v>0.12565000000000001</v>
+      </c>
+      <c r="D224" s="4">
+        <f t="shared" si="19"/>
+        <v>0.51486486486486482</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B225">
+        <v>1683</v>
+      </c>
+      <c r="D225" s="4"/>
+    </row>
+    <row r="226" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B226">
+        <v>1235</v>
+      </c>
+      <c r="D226" s="4"/>
+    </row>
+    <row r="227" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B227">
+        <v>0.94</v>
+      </c>
+      <c r="C227">
+        <v>0.9355</v>
+      </c>
+      <c r="D227" s="4">
+        <f t="shared" ref="D227:D231" si="20">ABS(C227-B227)/B227</f>
+        <v>4.7872340425531368E-3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B228">
+        <v>0.94</v>
+      </c>
+      <c r="D228" s="4"/>
+    </row>
+    <row r="229" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B229">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D229" s="4"/>
+    </row>
+    <row r="230" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B230" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C230">
+        <v>10219.5</v>
+      </c>
+      <c r="D230" s="4">
+        <f>ABS(C230-B230)/B230</f>
+        <v>2.1950000000000001E-2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D231" s="4">
+        <f>AVERAGE(D213:D230)</f>
+        <v>0.29318340911084773</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B232" s="16"/>
+      <c r="C232" s="16"/>
+      <c r="D232" s="16"/>
+    </row>
+    <row r="233" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B234" s="3">
+        <v>2340000000000</v>
+      </c>
+      <c r="C234" s="3"/>
+      <c r="D234" s="4">
+        <f>ABS(C234-B234)/B234</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B235" s="3">
+        <v>181000</v>
+      </c>
+      <c r="C235" s="3"/>
+      <c r="D235" s="4">
+        <f t="shared" ref="D235:D251" si="21">ABS(C235-B235)/B235</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B236">
+        <v>1</v>
+      </c>
+      <c r="D236" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B237" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D237" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B238" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="D238" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B239" s="3">
+        <v>4.405E-5</v>
+      </c>
+      <c r="C239" s="3"/>
+      <c r="D239" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B240" s="5">
+        <v>1080</v>
+      </c>
+      <c r="D240" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B241" s="5">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="D241" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B242">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="D242" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B243" s="5">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="D243" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B244">
+        <v>1041</v>
+      </c>
+      <c r="D244" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B245" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="D245" s="4">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B246">
+        <v>1683</v>
+      </c>
+      <c r="D246" s="4"/>
+    </row>
+    <row r="247" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A247" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B247">
+        <v>1235</v>
+      </c>
+      <c r="D247" s="4"/>
+    </row>
+    <row r="248" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A248" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B248">
+        <v>0.94</v>
+      </c>
+      <c r="D248" s="4">
+        <f t="shared" ref="D248:D252" si="22">ABS(C248-B248)/B248</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A249" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B249">
+        <v>0.94</v>
+      </c>
+      <c r="D249" s="4"/>
+    </row>
+    <row r="250" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B250">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D250" s="4"/>
+    </row>
+    <row r="251" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B251" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D251" s="4">
+        <f>ABS(C251-B251)/B251</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D252" s="4">
+        <f>AVERAGE(D234:D251)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="12">
+    <mergeCell ref="A211:D211"/>
+    <mergeCell ref="A232:D232"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A148:D148"/>
+    <mergeCell ref="A169:D169"/>
+    <mergeCell ref="A190:D190"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A85:D85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2912,6 +6088,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2926,6 +6103,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2940,6 +6118,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3245,6 +6424,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3491,6 +6671,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3840,6 +7021,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4097,6 +7279,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F20"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
rerun 2reactions 2mass tga
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="114">
   <si>
     <t>Input parameters</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Average</t>
   </si>
   <si>
-    <t>running_home</t>
-  </si>
-  <si>
     <t>running_office</t>
   </si>
   <si>
@@ -374,6 +371,12 @@
   </si>
   <si>
     <t>Good for low heat flux</t>
+  </si>
+  <si>
+    <t>8.29-250.02%</t>
+  </si>
+  <si>
+    <t>4.57-176.55%</t>
   </si>
 </sst>
 </file>
@@ -542,13 +545,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -836,11 +839,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,16 +862,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -881,16 +884,16 @@
         <v>48</v>
       </c>
       <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
         <v>107</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>108</v>
       </c>
-      <c r="F2" t="s">
-        <v>109</v>
-      </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H2" t="s">
         <v>45</v>
@@ -904,7 +907,7 @@
         <v>1.2545999999999999</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>34</v>
@@ -918,7 +921,7 @@
         <v>0.47799999999999998</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>30</v>
@@ -932,7 +935,7 @@
         <v>0.36809999999999998</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>30</v>
@@ -946,7 +949,7 @@
         <v>0.27350000000000002</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>30</v>
@@ -960,7 +963,7 @@
         <v>5.4800000000000001E-2</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>30</v>
@@ -974,7 +977,7 @@
         <v>0.47689999999999999</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>44</v>
@@ -988,7 +991,7 @@
         <v>0.1825</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>30</v>
@@ -1002,7 +1005,7 @@
         <v>0.66779999999999995</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>30</v>
@@ -1016,7 +1019,7 @@
         <v>0.66610000000000003</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>34</v>
@@ -1030,7 +1033,7 @@
         <v>0.32590000000000002</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>44</v>
@@ -1044,7 +1047,7 @@
         <v>0.29320000000000002</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>44</v>
@@ -1059,16 +1062,16 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1081,16 +1084,16 @@
         <v>48</v>
       </c>
       <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" t="s">
         <v>107</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>108</v>
       </c>
-      <c r="F16" t="s">
-        <v>109</v>
-      </c>
       <c r="G16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H16" t="s">
         <v>45</v>
@@ -1104,7 +1107,7 @@
         <v>0.80300000000000005</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17">
         <v>5.67571366083333E-2</v>
@@ -1131,7 +1134,7 @@
         <v>0.28520000000000001</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18">
         <v>4.8458532313333302E-2</v>
@@ -1166,7 +1169,7 @@
         <v>0.75639999999999996</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D20">
         <v>4.2059522093333301E-2</v>
@@ -1193,7 +1196,7 @@
         <v>0.3952</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21">
         <v>1.02705163433333E-2</v>
@@ -1220,7 +1223,7 @@
         <v>0.4516</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22">
         <v>9.9509812685000004E-2</v>
@@ -1247,7 +1250,7 @@
         <v>0.42709999999999998</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23">
         <v>3.7636890781666599E-2</v>
@@ -1274,7 +1277,7 @@
         <v>0.64629999999999999</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24">
         <v>1.73429586583333E-2</v>
@@ -1301,7 +1304,7 @@
         <v>0.22270000000000001</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D25">
         <v>8.0970326166666603E-4</v>
@@ -1321,16 +1324,16 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1343,16 +1346,16 @@
         <v>48</v>
       </c>
       <c r="D27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" t="s">
         <v>107</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>108</v>
       </c>
-      <c r="F27" t="s">
-        <v>109</v>
-      </c>
       <c r="G27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H27" t="s">
         <v>45</v>
@@ -1366,7 +1369,7 @@
         <v>0.2021</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D28">
         <v>1.8085282163333299E-2</v>
@@ -1393,7 +1396,7 @@
         <v>0.74260000000000004</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D29">
         <v>0.17225772079499899</v>
@@ -1420,7 +1423,7 @@
         <v>0.34789999999999999</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D30">
         <v>6.2844071950000002E-3</v>
@@ -1447,7 +1450,7 @@
         <v>0.71889999999999998</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D31">
         <v>0.17473352948333301</v>
@@ -1470,8 +1473,27 @@
       <c r="A32" t="s">
         <v>51</v>
       </c>
+      <c r="B32" s="4">
+        <v>0.61560000000000004</v>
+      </c>
+      <c r="C32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32">
+        <v>0.13735832918833299</v>
+      </c>
+      <c r="E32">
+        <v>4.6736408083333401E-3</v>
+      </c>
+      <c r="F32">
+        <v>3.4981999833333202E-3</v>
+      </c>
+      <c r="G32">
+        <f>AVERAGE(D32:F32)</f>
+        <v>4.8510056659999884E-2</v>
+      </c>
       <c r="H32" s="13" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1479,7 +1501,7 @@
         <v>52</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1490,7 +1512,7 @@
         <v>0.87809999999999999</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34">
         <v>3.7005961699999898E-3</v>
@@ -1506,7 +1528,7 @@
         <v>9.6914271372222031E-3</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1517,7 +1539,7 @@
         <v>0.2026</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35">
         <v>6.9319584164999906E-2</v>
@@ -1540,8 +1562,27 @@
       <c r="A36" t="s">
         <v>47</v>
       </c>
+      <c r="B36" s="4">
+        <v>0.69750000000000001</v>
+      </c>
+      <c r="C36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36">
+        <v>4.1863751386666599E-2</v>
+      </c>
+      <c r="E36">
+        <v>1.2767784558333301E-2</v>
+      </c>
+      <c r="F36">
+        <v>1.8572534416666599E-2</v>
+      </c>
+      <c r="G36">
+        <f>AVERAGE(D36:F36)</f>
+        <v>2.4401356787222165E-2</v>
+      </c>
       <c r="H36" s="16" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1553,16 +1594,16 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1575,16 +1616,16 @@
         <v>48</v>
       </c>
       <c r="D39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" t="s">
         <v>107</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>108</v>
       </c>
-      <c r="F39" t="s">
-        <v>109</v>
-      </c>
       <c r="G39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H39" t="s">
         <v>45</v>
@@ -1615,8 +1656,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
-        <v>110</v>
+      <c r="A44" s="20" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3178,12 +3219,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3432,7 +3473,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>0.73380000000000001</v>
@@ -3467,12 +3508,12 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
     </row>
     <row r="23" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -3721,7 +3762,7 @@
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40">
         <v>0.73380000000000001</v>
@@ -3756,12 +3797,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
     </row>
     <row r="44" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -4001,7 +4042,7 @@
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61">
         <v>0.73380000000000001</v>
@@ -4033,12 +4074,12 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
     </row>
     <row r="65" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
@@ -4278,7 +4319,7 @@
     </row>
     <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B82">
         <v>0.73380000000000001</v>
@@ -4310,12 +4351,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B85" s="20"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="20"/>
+      <c r="A85" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
     </row>
     <row r="86" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
@@ -4555,7 +4596,7 @@
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B103">
         <v>0.73380000000000001</v>
@@ -4587,12 +4628,12 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B106" s="20"/>
-      <c r="C106" s="20"/>
-      <c r="D106" s="20"/>
+      <c r="A106" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B106" s="22"/>
+      <c r="C106" s="22"/>
+      <c r="D106" s="22"/>
     </row>
     <row r="107" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
@@ -4832,7 +4873,7 @@
     </row>
     <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B124">
         <v>0.73380000000000001</v>
@@ -4864,12 +4905,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B127" s="20"/>
-      <c r="C127" s="20"/>
-      <c r="D127" s="20"/>
+      <c r="A127" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B127" s="22"/>
+      <c r="C127" s="22"/>
+      <c r="D127" s="22"/>
     </row>
     <row r="128" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
@@ -5109,7 +5150,7 @@
     </row>
     <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B145">
         <v>0.73380000000000001</v>
@@ -5141,12 +5182,12 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="20" t="s">
+      <c r="A148" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B148" s="20"/>
-      <c r="C148" s="20"/>
-      <c r="D148" s="20"/>
+      <c r="B148" s="22"/>
+      <c r="C148" s="22"/>
+      <c r="D148" s="22"/>
     </row>
     <row r="149" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
@@ -5386,7 +5427,7 @@
     </row>
     <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B166">
         <v>0.73380000000000001</v>
@@ -5418,12 +5459,12 @@
       </c>
     </row>
     <row r="169" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="20" t="s">
+      <c r="A169" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B169" s="20"/>
-      <c r="C169" s="20"/>
-      <c r="D169" s="20"/>
+      <c r="B169" s="22"/>
+      <c r="C169" s="22"/>
+      <c r="D169" s="22"/>
     </row>
     <row r="170" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
@@ -5663,7 +5704,7 @@
     </row>
     <row r="187" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B187">
         <v>0.73380000000000001</v>
@@ -5695,12 +5736,12 @@
       </c>
     </row>
     <row r="190" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B190" s="20"/>
-      <c r="C190" s="20"/>
-      <c r="D190" s="20"/>
+      <c r="A190" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B190" s="22"/>
+      <c r="C190" s="22"/>
+      <c r="D190" s="22"/>
     </row>
     <row r="191" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
@@ -5940,7 +5981,7 @@
     </row>
     <row r="208" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B208">
         <v>0.73380000000000001</v>
@@ -5972,12 +6013,12 @@
       </c>
     </row>
     <row r="211" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B211" s="20"/>
-      <c r="C211" s="20"/>
-      <c r="D211" s="20"/>
+      <c r="A211" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B211" s="22"/>
+      <c r="C211" s="22"/>
+      <c r="D211" s="22"/>
     </row>
     <row r="212" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
@@ -6217,7 +6258,7 @@
     </row>
     <row r="229" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B229">
         <v>0.73380000000000001</v>
@@ -6249,12 +6290,12 @@
       </c>
     </row>
     <row r="232" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B232" s="20"/>
-      <c r="C232" s="20"/>
-      <c r="D232" s="20"/>
+      <c r="A232" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B232" s="22"/>
+      <c r="C232" s="22"/>
+      <c r="D232" s="22"/>
     </row>
     <row r="233" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
@@ -6458,7 +6499,7 @@
     </row>
     <row r="250" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B250">
         <v>0.73380000000000001</v>
@@ -6488,6 +6529,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A85:D85"/>
     <mergeCell ref="A211:D211"/>
     <mergeCell ref="A232:D232"/>
     <mergeCell ref="A106:D106"/>
@@ -6495,11 +6541,6 @@
     <mergeCell ref="A148:D148"/>
     <mergeCell ref="A169:D169"/>
     <mergeCell ref="A190:D190"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A85:D85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6513,8 +6554,8 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:D26"/>
+    <sheetView topLeftCell="A22" workbookViewId="1">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6523,12 +6564,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6546,7 +6587,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3">
         <v>2340000000000</v>
@@ -6561,7 +6602,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3">
         <v>75000000000000</v>
@@ -6636,7 +6677,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="3">
         <v>181000</v>
@@ -6651,7 +6692,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3">
         <v>193000</v>
@@ -6666,7 +6707,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="3">
         <v>100000</v>
@@ -6681,7 +6722,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3">
         <v>200000</v>
@@ -6711,7 +6752,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>0.75</v>
@@ -6726,7 +6767,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15">
         <v>0.5</v>
@@ -6825,7 +6866,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -6840,7 +6881,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23">
         <v>1.5</v>
@@ -6889,12 +6930,12 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
+      <c r="A27" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
     </row>
     <row r="28" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -6912,7 +6953,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29" s="3">
         <v>2340000000000</v>
@@ -6927,7 +6968,7 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="3">
         <v>75000000000000</v>
@@ -7002,7 +7043,7 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" s="3">
         <v>181000</v>
@@ -7017,7 +7058,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="3">
         <v>193000</v>
@@ -7032,7 +7073,7 @@
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" s="3">
         <v>100000</v>
@@ -7047,7 +7088,7 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="3">
         <v>200000</v>
@@ -7077,7 +7118,7 @@
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40">
         <v>0.75</v>
@@ -7092,7 +7133,7 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41">
         <v>0.5</v>
@@ -7191,7 +7232,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -7206,7 +7247,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B49">
         <v>1.5</v>
@@ -7255,12 +7296,12 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="20" t="s">
+      <c r="A53" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
     </row>
     <row r="54" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
@@ -7278,7 +7319,7 @@
     </row>
     <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" s="3">
         <v>2340000000000</v>
@@ -7291,7 +7332,7 @@
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B56" s="3">
         <v>75000000000000</v>
@@ -7352,7 +7393,7 @@
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61" s="3">
         <v>181000</v>
@@ -7365,7 +7406,7 @@
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B62" s="3">
         <v>193000</v>
@@ -7378,7 +7419,7 @@
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B63" s="3">
         <v>100000</v>
@@ -7390,7 +7431,7 @@
     </row>
     <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B64" s="3">
         <v>200000</v>
@@ -7414,7 +7455,7 @@
     </row>
     <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66">
         <v>0.75</v>
@@ -7426,7 +7467,7 @@
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B67">
         <v>0.5</v>
@@ -7509,7 +7550,7 @@
     </row>
     <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -7521,7 +7562,7 @@
     </row>
     <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B75">
         <v>1.5</v>
@@ -7561,12 +7602,12 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="20" t="s">
+      <c r="A79" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
     </row>
     <row r="80" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
@@ -7584,7 +7625,7 @@
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="3">
         <v>2340000000000</v>
@@ -7599,7 +7640,7 @@
     </row>
     <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82" s="3">
         <v>75000000000000</v>
@@ -7674,7 +7715,7 @@
     </row>
     <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B87" s="3">
         <v>181000</v>
@@ -7689,7 +7730,7 @@
     </row>
     <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B88" s="3">
         <v>193000</v>
@@ -7704,7 +7745,7 @@
     </row>
     <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B89" s="3">
         <v>100000</v>
@@ -7719,7 +7760,7 @@
     </row>
     <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B90" s="3">
         <v>200000</v>
@@ -7749,7 +7790,7 @@
     </row>
     <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B92">
         <v>0.75</v>
@@ -7764,7 +7805,7 @@
     </row>
     <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B93">
         <v>0.5</v>
@@ -7863,7 +7904,7 @@
     </row>
     <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -7878,7 +7919,7 @@
     </row>
     <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B101">
         <v>1.5</v>
@@ -7927,12 +7968,12 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B105" s="20"/>
-      <c r="C105" s="20"/>
-      <c r="D105" s="20"/>
+      <c r="A105" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B105" s="22"/>
+      <c r="C105" s="22"/>
+      <c r="D105" s="22"/>
     </row>
     <row r="106" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
@@ -7950,7 +7991,7 @@
     </row>
     <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B107" s="3">
         <v>2340000000000</v>
@@ -7965,7 +8006,7 @@
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B108" s="3">
         <v>75000000000000</v>
@@ -8040,7 +8081,7 @@
     </row>
     <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B113" s="3">
         <v>181000</v>
@@ -8055,7 +8096,7 @@
     </row>
     <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B114" s="3">
         <v>193000</v>
@@ -8070,7 +8111,7 @@
     </row>
     <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B115" s="3">
         <v>100000</v>
@@ -8085,7 +8126,7 @@
     </row>
     <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B116" s="3">
         <v>200000</v>
@@ -8115,7 +8156,7 @@
     </row>
     <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B118">
         <v>0.75</v>
@@ -8130,7 +8171,7 @@
     </row>
     <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B119">
         <v>0.5</v>
@@ -8229,7 +8270,7 @@
     </row>
     <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -8244,7 +8285,7 @@
     </row>
     <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B127">
         <v>1.5</v>
@@ -8293,12 +8334,12 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="20" t="s">
+      <c r="A131" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B131" s="20"/>
-      <c r="C131" s="20"/>
-      <c r="D131" s="20"/>
+      <c r="B131" s="22"/>
+      <c r="C131" s="22"/>
+      <c r="D131" s="22"/>
     </row>
     <row r="132" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
@@ -8316,7 +8357,7 @@
     </row>
     <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B133" s="3">
         <v>2340000000000</v>
@@ -8331,7 +8372,7 @@
     </row>
     <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B134" s="3">
         <v>75000000000000</v>
@@ -8406,7 +8447,7 @@
     </row>
     <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B139" s="3">
         <v>181000</v>
@@ -8421,7 +8462,7 @@
     </row>
     <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B140" s="3">
         <v>193000</v>
@@ -8436,7 +8477,7 @@
     </row>
     <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B141" s="3">
         <v>100000</v>
@@ -8451,7 +8492,7 @@
     </row>
     <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B142" s="3">
         <v>200000</v>
@@ -8481,7 +8522,7 @@
     </row>
     <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B144">
         <v>0.75</v>
@@ -8496,7 +8537,7 @@
     </row>
     <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B145">
         <v>0.5</v>
@@ -8595,7 +8636,7 @@
     </row>
     <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B152">
         <v>1</v>
@@ -8610,7 +8651,7 @@
     </row>
     <row r="153" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B153">
         <v>1.5</v>
@@ -8659,12 +8700,12 @@
       </c>
     </row>
     <row r="157" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="20" t="s">
+      <c r="A157" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B157" s="20"/>
-      <c r="C157" s="20"/>
-      <c r="D157" s="20"/>
+      <c r="B157" s="22"/>
+      <c r="C157" s="22"/>
+      <c r="D157" s="22"/>
     </row>
     <row r="158" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
@@ -8682,7 +8723,7 @@
     </row>
     <row r="159" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B159" s="3">
         <v>2340000000000</v>
@@ -8697,7 +8738,7 @@
     </row>
     <row r="160" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B160" s="3">
         <v>75000000000000</v>
@@ -8772,7 +8813,7 @@
     </row>
     <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B165" s="3">
         <v>181000</v>
@@ -8787,7 +8828,7 @@
     </row>
     <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B166" s="3">
         <v>193000</v>
@@ -8802,7 +8843,7 @@
     </row>
     <row r="167" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B167" s="3">
         <v>100000</v>
@@ -8817,7 +8858,7 @@
     </row>
     <row r="168" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B168" s="3">
         <v>200000</v>
@@ -8847,7 +8888,7 @@
     </row>
     <row r="170" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B170">
         <v>0.75</v>
@@ -8862,7 +8903,7 @@
     </row>
     <row r="171" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B171">
         <v>0.5</v>
@@ -8961,7 +9002,7 @@
     </row>
     <row r="178" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B178">
         <v>1</v>
@@ -8976,7 +9017,7 @@
     </row>
     <row r="179" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B179">
         <v>1.5</v>
@@ -9025,12 +9066,12 @@
       </c>
     </row>
     <row r="183" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B183" s="20"/>
-      <c r="C183" s="20"/>
-      <c r="D183" s="20"/>
+      <c r="A183" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B183" s="22"/>
+      <c r="C183" s="22"/>
+      <c r="D183" s="22"/>
     </row>
     <row r="184" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
@@ -9048,7 +9089,7 @@
     </row>
     <row r="185" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B185" s="3">
         <v>2340000000000</v>
@@ -9063,7 +9104,7 @@
     </row>
     <row r="186" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B186" s="3">
         <v>75000000000000</v>
@@ -9138,7 +9179,7 @@
     </row>
     <row r="191" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B191" s="3">
         <v>181000</v>
@@ -9153,7 +9194,7 @@
     </row>
     <row r="192" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B192" s="3">
         <v>193000</v>
@@ -9168,7 +9209,7 @@
     </row>
     <row r="193" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B193" s="3">
         <v>100000</v>
@@ -9183,7 +9224,7 @@
     </row>
     <row r="194" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B194" s="3">
         <v>200000</v>
@@ -9213,7 +9254,7 @@
     </row>
     <row r="196" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B196">
         <v>0.75</v>
@@ -9228,7 +9269,7 @@
     </row>
     <row r="197" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B197">
         <v>0.5</v>
@@ -9327,7 +9368,7 @@
     </row>
     <row r="204" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B204">
         <v>1</v>
@@ -9342,7 +9383,7 @@
     </row>
     <row r="205" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B205">
         <v>1.5</v>
@@ -9391,12 +9432,12 @@
       </c>
     </row>
     <row r="209" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B209" s="20"/>
-      <c r="C209" s="20"/>
-      <c r="D209" s="20"/>
+      <c r="A209" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B209" s="22"/>
+      <c r="C209" s="22"/>
+      <c r="D209" s="22"/>
     </row>
     <row r="210" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
@@ -9414,7 +9455,7 @@
     </row>
     <row r="211" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B211" s="3">
         <v>2340000000000</v>
@@ -9429,7 +9470,7 @@
     </row>
     <row r="212" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B212" s="3">
         <v>75000000000000</v>
@@ -9504,7 +9545,7 @@
     </row>
     <row r="217" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B217" s="3">
         <v>181000</v>
@@ -9519,7 +9560,7 @@
     </row>
     <row r="218" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B218" s="3">
         <v>193000</v>
@@ -9534,7 +9575,7 @@
     </row>
     <row r="219" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B219" s="3">
         <v>100000</v>
@@ -9549,7 +9590,7 @@
     </row>
     <row r="220" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B220" s="3">
         <v>200000</v>
@@ -9579,7 +9620,7 @@
     </row>
     <row r="222" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B222">
         <v>0.75</v>
@@ -9594,7 +9635,7 @@
     </row>
     <row r="223" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B223">
         <v>0.5</v>
@@ -9693,7 +9734,7 @@
     </row>
     <row r="230" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B230">
         <v>1</v>
@@ -9708,7 +9749,7 @@
     </row>
     <row r="231" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B231">
         <v>1.5</v>
@@ -9776,11 +9817,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D279"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="K183" sqref="K183"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="1">
-      <selection activeCell="C226" sqref="C226"/>
+    <sheetView topLeftCell="A94" workbookViewId="1">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9789,12 +9830,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9812,7 +9853,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3">
         <v>2340000000000</v>
@@ -9827,7 +9868,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3">
         <v>75000000000000</v>
@@ -9842,7 +9883,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="3">
         <v>9200000000000</v>
@@ -9917,7 +9958,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="3">
         <v>181000</v>
@@ -9932,7 +9973,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" s="3">
         <v>193000</v>
@@ -9947,7 +9988,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" s="3">
         <v>175000</v>
@@ -9962,7 +10003,7 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3">
         <v>100000</v>
@@ -9977,7 +10018,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="3">
         <v>200000</v>
@@ -9992,7 +10033,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="3">
         <v>400000</v>
@@ -10022,7 +10063,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17">
         <v>0.75</v>
@@ -10037,7 +10078,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18">
         <v>0.5</v>
@@ -10052,7 +10093,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19">
         <v>0.3</v>
@@ -10151,7 +10192,7 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -10166,7 +10207,7 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27">
         <v>1.5</v>
@@ -10181,7 +10222,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -10230,12 +10271,12 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
     </row>
     <row r="33" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -10253,7 +10294,7 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="3">
         <v>2340000000000</v>
@@ -10268,7 +10309,7 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B35" s="3">
         <v>75000000000000</v>
@@ -10283,7 +10324,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" s="3">
         <v>9200000000000</v>
@@ -10358,7 +10399,7 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" s="3">
         <v>181000</v>
@@ -10373,7 +10414,7 @@
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" s="3">
         <v>193000</v>
@@ -10388,7 +10429,7 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B43" s="3">
         <v>175000</v>
@@ -10403,7 +10444,7 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44" s="3">
         <v>100000</v>
@@ -10418,7 +10459,7 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" s="3">
         <v>200000</v>
@@ -10433,7 +10474,7 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" s="3">
         <v>400000</v>
@@ -10463,7 +10504,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48">
         <v>0.75</v>
@@ -10478,7 +10519,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B49">
         <v>0.5</v>
@@ -10493,7 +10534,7 @@
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50">
         <v>0.3</v>
@@ -10592,7 +10633,7 @@
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -10607,7 +10648,7 @@
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B58">
         <v>1.5</v>
@@ -10622,7 +10663,7 @@
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -10671,12 +10712,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="20" t="s">
+      <c r="A63" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
     </row>
     <row r="64" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
@@ -10694,7 +10735,7 @@
     </row>
     <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="3">
         <v>2340000000000</v>
@@ -10709,7 +10750,7 @@
     </row>
     <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B66" s="3">
         <v>75000000000000</v>
@@ -10724,7 +10765,7 @@
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B67" s="3">
         <v>9200000000000</v>
@@ -10799,7 +10840,7 @@
     </row>
     <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B72" s="3">
         <v>181000</v>
@@ -10814,7 +10855,7 @@
     </row>
     <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B73" s="3">
         <v>193000</v>
@@ -10829,7 +10870,7 @@
     </row>
     <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B74" s="3">
         <v>175000</v>
@@ -10844,7 +10885,7 @@
     </row>
     <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B75" s="3">
         <v>100000</v>
@@ -10859,7 +10900,7 @@
     </row>
     <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" s="3">
         <v>200000</v>
@@ -10874,7 +10915,7 @@
     </row>
     <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B77" s="3">
         <v>400000</v>
@@ -10904,7 +10945,7 @@
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79">
         <v>0.75</v>
@@ -10919,7 +10960,7 @@
     </row>
     <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80">
         <v>0.5</v>
@@ -10934,7 +10975,7 @@
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B81">
         <v>0.3</v>
@@ -11033,7 +11074,7 @@
     </row>
     <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -11048,7 +11089,7 @@
     </row>
     <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B89">
         <v>1.5</v>
@@ -11063,7 +11104,7 @@
     </row>
     <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -11112,12 +11153,12 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="20" t="s">
+      <c r="A94" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B94" s="20"/>
-      <c r="C94" s="20"/>
-      <c r="D94" s="20"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="22"/>
     </row>
     <row r="95" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
@@ -11135,7 +11176,7 @@
     </row>
     <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B96" s="3">
         <v>2340000000000</v>
@@ -11150,7 +11191,7 @@
     </row>
     <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B97" s="3">
         <v>75000000000000</v>
@@ -11165,7 +11206,7 @@
     </row>
     <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98" s="3">
         <v>9200000000000</v>
@@ -11240,7 +11281,7 @@
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B103" s="3">
         <v>181000</v>
@@ -11255,7 +11296,7 @@
     </row>
     <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B104" s="3">
         <v>193000</v>
@@ -11270,7 +11311,7 @@
     </row>
     <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B105" s="3">
         <v>175000</v>
@@ -11285,7 +11326,7 @@
     </row>
     <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B106" s="3">
         <v>100000</v>
@@ -11300,7 +11341,7 @@
     </row>
     <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B107" s="3">
         <v>200000</v>
@@ -11315,7 +11356,7 @@
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B108" s="3">
         <v>400000</v>
@@ -11345,7 +11386,7 @@
     </row>
     <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B110">
         <v>0.75</v>
@@ -11360,7 +11401,7 @@
     </row>
     <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B111">
         <v>0.5</v>
@@ -11375,7 +11416,7 @@
     </row>
     <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B112">
         <v>0.3</v>
@@ -11474,7 +11515,7 @@
     </row>
     <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -11489,7 +11530,7 @@
     </row>
     <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B120">
         <v>1.5</v>
@@ -11504,7 +11545,7 @@
     </row>
     <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B121">
         <v>3</v>
@@ -11553,12 +11594,12 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="20" t="s">
+      <c r="A125" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B125" s="20"/>
-      <c r="C125" s="20"/>
-      <c r="D125" s="20"/>
+      <c r="B125" s="22"/>
+      <c r="C125" s="22"/>
+      <c r="D125" s="22"/>
     </row>
     <row r="126" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
@@ -11576,47 +11617,47 @@
     </row>
     <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B127" s="3">
         <v>2340000000000</v>
       </c>
       <c r="C127" s="3">
-        <v>4140000000000</v>
+        <v>2110000000000</v>
       </c>
       <c r="D127" s="4">
         <f t="shared" ref="D127:D133" si="16">ABS(C127-B127)/B127</f>
-        <v>0.76923076923076927</v>
+        <v>9.8290598290598288E-2</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B128" s="3">
         <v>75000000000000</v>
       </c>
       <c r="C128" s="3">
-        <v>106000000000000</v>
+        <v>70800000000000</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="16"/>
-        <v>0.41333333333333333</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B129" s="3">
         <v>9200000000000</v>
       </c>
       <c r="C129" s="3">
-        <v>16600000000000</v>
+        <v>9620000000000</v>
       </c>
       <c r="D129" s="4">
         <f t="shared" si="16"/>
-        <v>0.80434782608695654</v>
+        <v>4.5652173913043478E-2</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11627,11 +11668,11 @@
         <v>1080</v>
       </c>
       <c r="C130">
-        <v>1595.86</v>
+        <v>1362.4</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="16"/>
-        <v>0.47764814814814804</v>
+        <v>0.26148148148148159</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11642,11 +11683,11 @@
         <v>1041</v>
       </c>
       <c r="C131">
-        <v>2035.33</v>
+        <v>2551.6</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="16"/>
-        <v>0.95516810758885684</v>
+        <v>1.4511047070124878</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -11657,11 +11698,11 @@
         <v>4.5199999999999997E-2</v>
       </c>
       <c r="C132">
-        <v>8.5800000000000001E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="16"/>
-        <v>0.8982300884955754</v>
+        <v>1.7654867256637172</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -11672,101 +11713,101 @@
         <v>0.25900000000000001</v>
       </c>
       <c r="C133">
-        <v>0.49099999999999999</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="D133" s="4">
         <f t="shared" si="16"/>
-        <v>0.89575289575289563</v>
+        <v>0.79536679536679544</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B134" s="3">
         <v>181000</v>
       </c>
       <c r="C134" s="3">
-        <v>209000</v>
+        <v>306000</v>
       </c>
       <c r="D134" s="4">
         <f t="shared" ref="D134" si="17">ABS(C134-B134)/B134</f>
-        <v>0.15469613259668508</v>
+        <v>0.69060773480662985</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B135" s="3">
         <v>193000</v>
       </c>
       <c r="C135" s="3">
-        <v>146000</v>
+        <v>159000</v>
       </c>
       <c r="D135" s="4">
         <f t="shared" ref="D135:D144" si="18">ABS(C135-B135)/B135</f>
-        <v>0.24352331606217617</v>
+        <v>0.17616580310880828</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B136" s="3">
         <v>175000</v>
       </c>
       <c r="C136" s="3">
-        <v>261000</v>
+        <v>216000</v>
       </c>
       <c r="D136" s="4">
         <f t="shared" si="18"/>
-        <v>0.49142857142857144</v>
+        <v>0.23428571428571429</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B137" s="3">
         <v>100000</v>
       </c>
       <c r="C137">
-        <v>220040</v>
+        <v>208191</v>
       </c>
       <c r="D137" s="4">
         <f t="shared" si="18"/>
-        <v>1.2003999999999999</v>
+        <v>1.0819099999999999</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B138" s="3">
         <v>200000</v>
       </c>
       <c r="C138">
-        <v>433347</v>
+        <v>342383</v>
       </c>
       <c r="D138" s="4">
         <f t="shared" si="18"/>
-        <v>1.1667350000000001</v>
+        <v>0.71191499999999996</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B139" s="3">
         <v>400000</v>
       </c>
       <c r="C139">
-        <v>832306</v>
+        <v>1001190.5</v>
       </c>
       <c r="D139" s="4">
         <f t="shared" si="18"/>
-        <v>1.080765</v>
+        <v>1.5029762499999999</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11777,56 +11818,56 @@
         <v>10000</v>
       </c>
       <c r="C140">
-        <v>26063.3</v>
+        <v>14034</v>
       </c>
       <c r="D140" s="4">
         <f t="shared" si="18"/>
-        <v>1.60633</v>
+        <v>0.40339999999999998</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B141">
         <v>0.75</v>
       </c>
       <c r="C141">
-        <v>0.4607</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="D141" s="4">
         <f t="shared" si="18"/>
-        <v>0.38573333333333332</v>
+        <v>0.20400000000000004</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B142">
         <v>0.5</v>
       </c>
       <c r="C142">
-        <v>0.43859999999999999</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="D142" s="4">
         <f t="shared" si="18"/>
-        <v>0.12280000000000002</v>
+        <v>0.10399999999999998</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B143">
         <v>0.3</v>
       </c>
       <c r="C143">
-        <v>0.49209999999999998</v>
+        <v>0.52</v>
       </c>
       <c r="D143" s="4">
         <f t="shared" si="18"/>
-        <v>0.64033333333333331</v>
+        <v>0.7333333333333335</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11837,11 +11878,11 @@
         <v>0.94</v>
       </c>
       <c r="C144">
-        <v>0.65400000000000003</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="D144" s="4">
         <f t="shared" si="18"/>
-        <v>0.30425531914893611</v>
+        <v>0.1744680851063829</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11861,11 +11902,11 @@
         <v>0.312</v>
       </c>
       <c r="C146">
-        <v>0.38700000000000001</v>
+        <v>0.27950000000000003</v>
       </c>
       <c r="D146" s="4">
         <f>ABS(C146-B146)/B146</f>
-        <v>0.24038461538461542</v>
+        <v>0.10416666666666659</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11876,11 +11917,11 @@
         <v>9.4899999999999998E-2</v>
       </c>
       <c r="C147">
-        <v>0.152</v>
+        <v>8.3650000000000002E-2</v>
       </c>
       <c r="D147" s="4">
         <f>ABS(C147-B147)/B147</f>
-        <v>0.60168598524762906</v>
+        <v>0.11854583772391988</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -11891,11 +11932,11 @@
         <v>4.405E-5</v>
       </c>
       <c r="C148" s="3">
-        <v>6.4197999999999998E-5</v>
+        <v>7.6000000000000004E-5</v>
       </c>
       <c r="D148" s="4">
         <f>ABS(C148-B148)/B148</f>
-        <v>0.45738933030646989</v>
+        <v>0.72531214528944388</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -11906,56 +11947,56 @@
         <v>2.8299999999999999E-4</v>
       </c>
       <c r="C149" s="3">
-        <v>5.0370000000000005E-4</v>
+        <v>6.4499999999999996E-4</v>
       </c>
       <c r="D149" s="4">
         <f>ABS(C149-B149)/B149</f>
-        <v>0.77985865724381642</v>
+        <v>1.2791519434628975</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B150">
         <v>1</v>
       </c>
       <c r="C150">
-        <v>2.2723</v>
+        <v>1.3</v>
       </c>
       <c r="D150" s="4">
         <f t="shared" ref="D150:D152" si="19">ABS(C150-B150)/B150</f>
-        <v>1.2723</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B151">
         <v>1.5</v>
       </c>
       <c r="C151">
-        <v>2.9805999999999999</v>
+        <v>2.95</v>
       </c>
       <c r="D151" s="4">
         <f t="shared" si="19"/>
-        <v>0.98706666666666665</v>
+        <v>0.96666666666666679</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B152">
         <v>3</v>
       </c>
       <c r="C152">
-        <v>6.0659999999999998</v>
+        <v>7.22</v>
       </c>
       <c r="D152" s="4">
         <f t="shared" si="19"/>
-        <v>1.022</v>
+        <v>1.4066666666666665</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11990,16 +12031,16 @@
       <c r="C155" s="18"/>
       <c r="D155" s="19">
         <f>AVERAGE(D127:D154)</f>
-        <v>0.71885585717555045</v>
+        <v>0.6156381731538102</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="20" t="s">
+      <c r="A156" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B156" s="20"/>
-      <c r="C156" s="20"/>
-      <c r="D156" s="20"/>
+      <c r="B156" s="22"/>
+      <c r="C156" s="22"/>
+      <c r="D156" s="22"/>
     </row>
     <row r="157" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
@@ -12017,7 +12058,7 @@
     </row>
     <row r="158" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B158" s="3">
         <v>2340000000000</v>
@@ -12032,7 +12073,7 @@
     </row>
     <row r="159" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B159" s="3">
         <v>75000000000000</v>
@@ -12047,7 +12088,7 @@
     </row>
     <row r="160" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B160" s="3">
         <v>9200000000000</v>
@@ -12122,7 +12163,7 @@
     </row>
     <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B165" s="3">
         <v>181000</v>
@@ -12137,7 +12178,7 @@
     </row>
     <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B166" s="3">
         <v>193000</v>
@@ -12152,7 +12193,7 @@
     </row>
     <row r="167" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B167" s="3">
         <v>175000</v>
@@ -12167,7 +12208,7 @@
     </row>
     <row r="168" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B168" s="3">
         <v>100000</v>
@@ -12182,7 +12223,7 @@
     </row>
     <row r="169" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B169" s="3">
         <v>200000</v>
@@ -12197,7 +12238,7 @@
     </row>
     <row r="170" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B170" s="3">
         <v>400000</v>
@@ -12227,7 +12268,7 @@
     </row>
     <row r="172" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B172">
         <v>0.75</v>
@@ -12242,7 +12283,7 @@
     </row>
     <row r="173" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B173">
         <v>0.5</v>
@@ -12257,7 +12298,7 @@
     </row>
     <row r="174" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B174">
         <v>0.3</v>
@@ -12356,7 +12397,7 @@
     </row>
     <row r="181" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -12371,7 +12412,7 @@
     </row>
     <row r="182" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B182">
         <v>1.5</v>
@@ -12386,7 +12427,7 @@
     </row>
     <row r="183" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B183">
         <v>3</v>
@@ -12435,12 +12476,12 @@
       </c>
     </row>
     <row r="187" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B187" s="20"/>
-      <c r="C187" s="20"/>
-      <c r="D187" s="20"/>
+      <c r="A187" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B187" s="22"/>
+      <c r="C187" s="22"/>
+      <c r="D187" s="22"/>
     </row>
     <row r="188" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
@@ -12458,7 +12499,7 @@
     </row>
     <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B189" s="3">
         <v>2340000000000</v>
@@ -12473,7 +12514,7 @@
     </row>
     <row r="190" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B190" s="3">
         <v>75000000000000</v>
@@ -12488,7 +12529,7 @@
     </row>
     <row r="191" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B191" s="3">
         <v>9200000000000</v>
@@ -12563,7 +12604,7 @@
     </row>
     <row r="196" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B196" s="3">
         <v>181000</v>
@@ -12578,7 +12619,7 @@
     </row>
     <row r="197" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B197" s="3">
         <v>193000</v>
@@ -12593,7 +12634,7 @@
     </row>
     <row r="198" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B198" s="3">
         <v>175000</v>
@@ -12608,7 +12649,7 @@
     </row>
     <row r="199" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B199" s="3">
         <v>100000</v>
@@ -12623,7 +12664,7 @@
     </row>
     <row r="200" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B200" s="3">
         <v>200000</v>
@@ -12638,7 +12679,7 @@
     </row>
     <row r="201" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B201" s="3">
         <v>400000</v>
@@ -12668,7 +12709,7 @@
     </row>
     <row r="203" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B203">
         <v>0.75</v>
@@ -12683,7 +12724,7 @@
     </row>
     <row r="204" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B204">
         <v>0.5</v>
@@ -12698,7 +12739,7 @@
     </row>
     <row r="205" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B205">
         <v>0.3</v>
@@ -12797,7 +12838,7 @@
     </row>
     <row r="212" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B212">
         <v>1</v>
@@ -12812,7 +12853,7 @@
     </row>
     <row r="213" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B213">
         <v>1.5</v>
@@ -12827,7 +12868,7 @@
     </row>
     <row r="214" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B214">
         <v>3</v>
@@ -12876,12 +12917,12 @@
       </c>
     </row>
     <row r="218" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="20" t="s">
+      <c r="A218" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B218" s="20"/>
-      <c r="C218" s="20"/>
-      <c r="D218" s="20"/>
+      <c r="B218" s="22"/>
+      <c r="C218" s="22"/>
+      <c r="D218" s="22"/>
     </row>
     <row r="219" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
@@ -12899,7 +12940,7 @@
     </row>
     <row r="220" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B220" s="3">
         <v>2340000000000</v>
@@ -12914,7 +12955,7 @@
     </row>
     <row r="221" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B221" s="3">
         <v>75000000000000</v>
@@ -12929,7 +12970,7 @@
     </row>
     <row r="222" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B222" s="3">
         <v>9200000000000</v>
@@ -13004,7 +13045,7 @@
     </row>
     <row r="227" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B227" s="3">
         <v>181000</v>
@@ -13019,7 +13060,7 @@
     </row>
     <row r="228" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B228" s="3">
         <v>193000</v>
@@ -13034,7 +13075,7 @@
     </row>
     <row r="229" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B229" s="3">
         <v>175000</v>
@@ -13049,7 +13090,7 @@
     </row>
     <row r="230" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B230" s="3">
         <v>100000</v>
@@ -13064,7 +13105,7 @@
     </row>
     <row r="231" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B231" s="3">
         <v>200000</v>
@@ -13079,7 +13120,7 @@
     </row>
     <row r="232" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B232" s="3">
         <v>400000</v>
@@ -13109,7 +13150,7 @@
     </row>
     <row r="234" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B234">
         <v>0.75</v>
@@ -13124,7 +13165,7 @@
     </row>
     <row r="235" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B235">
         <v>0.5</v>
@@ -13139,7 +13180,7 @@
     </row>
     <row r="236" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B236">
         <v>0.3</v>
@@ -13238,7 +13279,7 @@
     </row>
     <row r="243" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B243">
         <v>1</v>
@@ -13253,7 +13294,7 @@
     </row>
     <row r="244" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B244">
         <v>1.5</v>
@@ -13268,7 +13309,7 @@
     </row>
     <row r="245" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B245">
         <v>3</v>
@@ -13317,12 +13358,12 @@
       </c>
     </row>
     <row r="249" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B249" s="20"/>
-      <c r="C249" s="20"/>
-      <c r="D249" s="20"/>
+      <c r="A249" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B249" s="22"/>
+      <c r="C249" s="22"/>
+      <c r="D249" s="22"/>
     </row>
     <row r="250" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
@@ -13340,47 +13381,47 @@
     </row>
     <row r="251" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B251" s="3">
         <v>2340000000000</v>
       </c>
       <c r="C251" s="3">
-        <v>2440000000000</v>
+        <v>1790000000000</v>
       </c>
       <c r="D251" s="4">
         <f t="shared" ref="D251:D257" si="32">ABS(C251-B251)/B251</f>
-        <v>4.2735042735042736E-2</v>
+        <v>0.23504273504273504</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B252" s="3">
         <v>75000000000000</v>
       </c>
       <c r="C252" s="3">
-        <v>75100000000000</v>
+        <v>95500000000000</v>
       </c>
       <c r="D252" s="4">
         <f t="shared" si="32"/>
-        <v>1.3333333333333333E-3</v>
+        <v>0.27333333333333332</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B253" s="3">
         <v>9200000000000</v>
       </c>
       <c r="C253" s="3">
-        <v>8920000000000</v>
+        <v>17200000000000</v>
       </c>
       <c r="D253" s="4">
         <f t="shared" si="32"/>
-        <v>3.0434782608695653E-2</v>
+        <v>0.86956521739130432</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13390,12 +13431,12 @@
       <c r="B254" s="5">
         <v>1080</v>
       </c>
-      <c r="C254">
-        <v>1064.33</v>
+      <c r="C254" s="5">
+        <v>873.28700000000003</v>
       </c>
       <c r="D254" s="4">
         <f t="shared" si="32"/>
-        <v>1.4509259259259326E-2</v>
+        <v>0.19140092592592589</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13405,12 +13446,12 @@
       <c r="B255">
         <v>1041</v>
       </c>
-      <c r="C255">
-        <v>1480.422</v>
+      <c r="C255" s="5">
+        <v>819.22500000000002</v>
       </c>
       <c r="D255" s="4">
         <f t="shared" si="32"/>
-        <v>0.42211527377521618</v>
+        <v>0.21304034582132564</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -13420,12 +13461,12 @@
       <c r="B256" s="5">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="C256">
-        <v>4.3490000000000001E-2</v>
+      <c r="C256" s="5">
+        <v>2.3900000000000001E-2</v>
       </c>
       <c r="D256" s="4">
         <f t="shared" si="32"/>
-        <v>3.7831858407079567E-2</v>
+        <v>0.4712389380530973</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -13435,102 +13476,102 @@
       <c r="B257" s="5">
         <v>0.25900000000000001</v>
       </c>
-      <c r="C257">
-        <v>0.3075</v>
+      <c r="C257" s="5">
+        <v>0.52449999999999997</v>
       </c>
       <c r="D257" s="4">
         <f t="shared" si="32"/>
-        <v>0.18725868725868722</v>
+        <v>1.0250965250965249</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B258" s="3">
         <v>181000</v>
       </c>
       <c r="C258" s="3">
-        <v>172000</v>
+        <v>166000</v>
       </c>
       <c r="D258" s="4">
         <f t="shared" ref="D258" si="33">ABS(C258-B258)/B258</f>
-        <v>4.9723756906077346E-2</v>
+        <v>8.2872928176795577E-2</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B259" s="3">
         <v>193000</v>
       </c>
       <c r="C259" s="3">
-        <v>179000</v>
+        <v>425000</v>
       </c>
       <c r="D259" s="4">
         <f t="shared" ref="D259:D268" si="34">ABS(C259-B259)/B259</f>
-        <v>7.2538860103626937E-2</v>
+        <v>1.2020725388601037</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B260" s="3">
         <v>175000</v>
       </c>
       <c r="C260" s="3">
-        <v>165000</v>
+        <v>266000</v>
       </c>
       <c r="D260" s="4">
         <f t="shared" si="34"/>
-        <v>5.7142857142857141E-2</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B261" s="3">
         <v>100000</v>
       </c>
-      <c r="C261">
-        <v>46032.4</v>
+      <c r="C261" s="3">
+        <v>290700</v>
       </c>
       <c r="D261" s="4">
         <f t="shared" si="34"/>
-        <v>0.53967599999999993</v>
+        <v>1.907</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B262" s="3">
         <v>200000</v>
       </c>
-      <c r="C262">
-        <v>346578.5</v>
+      <c r="C262" s="3">
+        <v>692109</v>
       </c>
       <c r="D262" s="4">
         <f t="shared" si="34"/>
-        <v>0.73289249999999995</v>
+        <v>2.4605450000000002</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B263" s="3">
         <v>400000</v>
       </c>
-      <c r="C263">
-        <v>410845.15</v>
+      <c r="C263" s="3">
+        <v>1400061</v>
       </c>
       <c r="D263" s="4">
         <f t="shared" si="34"/>
-        <v>2.7112875000000057E-2</v>
+        <v>2.5001525</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13540,57 +13581,57 @@
       <c r="B264" s="3">
         <v>10000</v>
       </c>
-      <c r="C264">
-        <v>26922.84</v>
+      <c r="C264" s="3">
+        <v>7697.5</v>
       </c>
       <c r="D264" s="4">
         <f t="shared" si="34"/>
-        <v>1.6922840000000001</v>
+        <v>0.23025000000000001</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B265">
         <v>0.75</v>
       </c>
-      <c r="C265">
-        <v>0.74450000000000005</v>
+      <c r="C265" s="3">
+        <v>0.43559999999999999</v>
       </c>
       <c r="D265" s="4">
         <f t="shared" si="34"/>
-        <v>7.3333333333332655E-3</v>
+        <v>0.41920000000000002</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B266">
         <v>0.5</v>
       </c>
-      <c r="C266">
-        <v>0.4889</v>
+      <c r="C266" s="3">
+        <v>0.629</v>
       </c>
       <c r="D266" s="4">
         <f t="shared" si="34"/>
-        <v>2.2199999999999998E-2</v>
+        <v>0.25800000000000001</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B267">
         <v>0.3</v>
       </c>
-      <c r="C267">
-        <v>0.31290000000000001</v>
+      <c r="C267" s="3">
+        <v>0.47499999999999998</v>
       </c>
       <c r="D267" s="4">
         <f t="shared" si="34"/>
-        <v>4.300000000000008E-2</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13600,12 +13641,12 @@
       <c r="B268">
         <v>0.94</v>
       </c>
-      <c r="C268">
-        <v>0.76859999999999995</v>
+      <c r="C268" s="3">
+        <v>0.80200000000000005</v>
       </c>
       <c r="D268" s="4">
         <f t="shared" si="34"/>
-        <v>0.1823404255319149</v>
+        <v>0.14680851063829778</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13624,12 +13665,12 @@
       <c r="B270" s="5">
         <v>0.312</v>
       </c>
-      <c r="C270">
-        <v>0.30059999999999998</v>
+      <c r="C270" s="3">
+        <v>0.2326</v>
       </c>
       <c r="D270" s="4">
         <f>ABS(C270-B270)/B270</f>
-        <v>3.653846153846161E-2</v>
+        <v>0.25448717948717947</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13639,12 +13680,12 @@
       <c r="B271">
         <v>9.4899999999999998E-2</v>
       </c>
-      <c r="C271">
-        <v>0.126</v>
+      <c r="C271" s="3">
+        <v>0.1439</v>
       </c>
       <c r="D271" s="4">
         <f>ABS(C271-B271)/B271</f>
-        <v>0.32771338250790311</v>
+        <v>0.51633298208640677</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -13655,11 +13696,11 @@
         <v>4.405E-5</v>
       </c>
       <c r="C272" s="3">
-        <v>3.3059999999999999E-5</v>
+        <v>5.1600000000000001E-5</v>
       </c>
       <c r="D272" s="4">
         <f>ABS(C272-B272)/B272</f>
-        <v>0.24948921679909197</v>
+        <v>0.17139614074914872</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -13670,56 +13711,56 @@
         <v>2.8299999999999999E-4</v>
       </c>
       <c r="C273" s="3">
-        <v>2.4439999999999998E-4</v>
+        <v>2.52E-4</v>
       </c>
       <c r="D273" s="4">
         <f>ABS(C273-B273)/B273</f>
-        <v>0.13639575971731455</v>
+        <v>0.10954063604240281</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B274">
         <v>1</v>
       </c>
-      <c r="C274">
-        <v>1.0389999999999999</v>
+      <c r="C274" s="3">
+        <v>1.65</v>
       </c>
       <c r="D274" s="4">
         <f t="shared" ref="D274:D276" si="35">ABS(C274-B274)/B274</f>
-        <v>3.8999999999999924E-2</v>
+        <v>0.64999999999999991</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B275">
         <v>1.5</v>
       </c>
-      <c r="C275">
-        <v>1.5569999999999999</v>
+      <c r="C275" s="3">
+        <v>4.5</v>
       </c>
       <c r="D275" s="4">
         <f t="shared" si="35"/>
-        <v>3.7999999999999957E-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B276">
         <v>3</v>
       </c>
-      <c r="C276">
-        <v>2.7749999999999999</v>
+      <c r="C276" s="3">
+        <v>3.4449999999999998</v>
       </c>
       <c r="D276" s="4">
         <f t="shared" si="35"/>
-        <v>7.5000000000000025E-2</v>
+        <v>0.14833333333333329</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13754,7 +13795,7 @@
       <c r="C279" s="18"/>
       <c r="D279" s="19">
         <f>AVERAGE(D251:D278)</f>
-        <v>0.20258398663831578</v>
+        <v>0.69756172413485018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>